<commit_message>
created DAO for tour, changed tour model
</commit_message>
<xml_diff>
--- a/docs/TimeTracking.xlsx
+++ b/docs/TimeTracking.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8ad2da8bf84885cf/Dokumente/GitHub/TourPlanner_Ortner_Szuesz/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FH Technikum Wien\Semster 4\Swen_Project\TourPlanner_Ortner_Szuesz\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{A6C857BF-3EEB-4E30-A6FF-427B75EDC3D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C71B1F80-2A6F-45E8-9462-F95DFB37705F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21E18F9-05A2-4F8A-B1A9-755C46B291E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="765" windowWidth="34980" windowHeight="20025" xr2:uid="{7D11CD6D-A168-461A-B814-780A183E0DF9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{7D11CD6D-A168-461A-B814-780A183E0DF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Tour-Planner Ortner &amp; Szüsz</t>
   </si>
@@ -50,6 +50,24 @@
   </si>
   <si>
     <t>Aufwand (h)</t>
+  </si>
+  <si>
+    <t>Basic UI layout</t>
+  </si>
+  <si>
+    <t>Finish basic UI layout and data binding</t>
+  </si>
+  <si>
+    <t>Define models, apply layered architecture</t>
+  </si>
+  <si>
+    <t>View Model Base, Relay Command</t>
+  </si>
+  <si>
+    <t>Created tour view model, basic business logic</t>
+  </si>
+  <si>
+    <t>Created database with demo data, database connection</t>
   </si>
 </sst>
 </file>
@@ -490,24 +508,24 @@
   <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="74.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" customWidth="1"/>
+    <col min="2" max="2" width="74.44140625" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
     </row>
-    <row r="3" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -518,7 +536,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>44619</v>
       </c>
@@ -529,185 +547,223 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-    </row>
-    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
+    <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>44676</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>44679</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>44680</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>44683</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>44685</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>44690</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>44691</v>
+      </c>
       <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-    </row>
-    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
       <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-    </row>
-    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
       <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-    </row>
-    <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="2"/>
       <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
       <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-    </row>
-    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
+      <c r="C15" s="4"/>
+    </row>
+    <row r="16" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="2"/>
       <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-    </row>
-    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
+      <c r="C16" s="4"/>
+    </row>
+    <row r="17" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
       <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-    </row>
-    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
+      <c r="C17" s="4"/>
+    </row>
+    <row r="18" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="2"/>
       <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-    </row>
-    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
+      <c r="C18" s="4"/>
+    </row>
+    <row r="19" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="2"/>
       <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-    </row>
-    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
+      <c r="C19" s="4"/>
+    </row>
+    <row r="20" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="2"/>
       <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-    </row>
-    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
+      <c r="C20" s="4"/>
+    </row>
+    <row r="21" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="2"/>
       <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-    </row>
-    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
+      <c r="C21" s="4"/>
+    </row>
+    <row r="22" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="2"/>
       <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-    </row>
-    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
+      <c r="C22" s="4"/>
+    </row>
+    <row r="23" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="2"/>
       <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-    </row>
-    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
+      <c r="C23" s="4"/>
+    </row>
+    <row r="24" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="2"/>
       <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
+      <c r="C24" s="4"/>
+    </row>
+    <row r="25" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="2"/>
       <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-    </row>
-    <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
+      <c r="C25" s="4"/>
+    </row>
+    <row r="26" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="2"/>
       <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-    </row>
-    <row r="27" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
+      <c r="C26" s="4"/>
+    </row>
+    <row r="27" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="2"/>
       <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-    </row>
-    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
+      <c r="C27" s="4"/>
+    </row>
+    <row r="28" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="2"/>
       <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-    </row>
-    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
+      <c r="C28" s="4"/>
+    </row>
+    <row r="29" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="2"/>
       <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-    </row>
-    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
+      <c r="C29" s="4"/>
+    </row>
+    <row r="30" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="2"/>
       <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-    </row>
-    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
+      <c r="C30" s="4"/>
+    </row>
+    <row r="31" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="2"/>
       <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-    </row>
-    <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
+      <c r="C31" s="4"/>
+    </row>
+    <row r="32" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="2"/>
       <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-    </row>
-    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
+      <c r="C32" s="4"/>
+    </row>
+    <row r="33" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="2"/>
       <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-    </row>
-    <row r="34" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
+      <c r="C33" s="4"/>
+    </row>
+    <row r="34" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="2"/>
       <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-    </row>
-    <row r="35" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
+      <c r="C34" s="4"/>
+    </row>
+    <row r="35" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="2"/>
       <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-    </row>
-    <row r="36" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
+      <c r="C35" s="4"/>
+    </row>
+    <row r="36" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="2"/>
       <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-    </row>
-    <row r="37" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
+      <c r="C36" s="4"/>
+    </row>
+    <row r="37" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="2"/>
       <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-    </row>
-    <row r="38" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="5"/>
+      <c r="C37" s="4"/>
+    </row>
+    <row r="38" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="2"/>
       <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
-    </row>
-    <row r="39" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="5"/>
+      <c r="C38" s="4"/>
+    </row>
+    <row r="39" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="2"/>
       <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-    </row>
-    <row r="40" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="5"/>
+      <c r="C39" s="4"/>
+    </row>
+    <row r="40" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="2"/>
       <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
+      <c r="C40" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
updating and deleting tour log
</commit_message>
<xml_diff>
--- a/docs/TimeTracking.xlsx
+++ b/docs/TimeTracking.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FH Technikum Wien\Semster 4\Swen_Project\TourPlanner_Ortner_Szuesz\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FH\SWEN\TourPlanner_Ortner_Szuesz\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21E18F9-05A2-4F8A-B1A9-755C46B291E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B9E9650-46E3-4475-9267-31416AD6FC5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{7D11CD6D-A168-461A-B814-780A183E0DF9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="37220" windowHeight="21820" xr2:uid="{7D11CD6D-A168-461A-B814-780A183E0DF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -35,23 +33,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Tour-Planner Ortner &amp; Szüsz</t>
   </si>
   <si>
-    <t>Datum</t>
-  </si>
-  <si>
-    <t>Beschreibung</t>
-  </si>
-  <si>
     <t>Github setup, Project setup, Basic application layout</t>
   </si>
   <si>
-    <t>Aufwand (h)</t>
-  </si>
-  <si>
     <t>Basic UI layout</t>
   </si>
   <si>
@@ -68,6 +57,42 @@
   </si>
   <si>
     <t>Created database with demo data, database connection</t>
+  </si>
+  <si>
+    <t>Created DAO for tour, changed tour model</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Time (h)</t>
+  </si>
+  <si>
+    <t>Dependency Injection, update UI when selected tour has changed</t>
+  </si>
+  <si>
+    <t>Create UI for route image, refactoring DAO for tours, finished http request for map quest</t>
+  </si>
+  <si>
+    <t>Created window for tour dialog, configuration with JSON file, create tour with route image</t>
+  </si>
+  <si>
+    <t>Added function to read route image file from file system, created datagrid for tour logs</t>
+  </si>
+  <si>
+    <t>Implemented bindings for tour information, tour SQL statements</t>
+  </si>
+  <si>
+    <t>Tour log SQL statements, create new tour logs for selected tour, created tour log dialog</t>
+  </si>
+  <si>
+    <t>SQL statements and functionality for updating and deleting of tours</t>
+  </si>
+  <si>
+    <t>SQL statements and functionality for updating and deleting of tour logs</t>
   </si>
 </sst>
 </file>
@@ -505,269 +530,328 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD90E2B8-0983-41CE-A418-47A70827F2D2}">
-  <dimension ref="A1:C40"/>
+  <dimension ref="B1:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.109375" customWidth="1"/>
-    <col min="2" max="2" width="74.44140625" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="4.7265625" customWidth="1"/>
+    <col min="2" max="2" width="13.08984375" customWidth="1"/>
+    <col min="3" max="3" width="82.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
       <c r="C1" s="6"/>
-    </row>
-    <row r="3" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="D1" s="6"/>
+    </row>
+    <row r="3" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B4" s="2">
+        <v>44619</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D4" s="4">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B5" s="2">
+        <v>44676</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D5" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B6" s="2">
+        <v>44679</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>44619</v>
-      </c>
-      <c r="B4" s="3" t="s">
+    <row r="7" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B7" s="2">
+        <v>44680</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B8" s="2">
+        <v>44683</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B9" s="2">
+        <v>44685</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B10" s="2">
+        <v>44690</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="4">
         <v>3</v>
       </c>
-      <c r="C4" s="4">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>44676</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="4">
+    </row>
+    <row r="11" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B11" s="2">
+        <v>44691</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B12" s="2">
+        <v>44692</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B13" s="2">
+        <v>44693</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>44679</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="4">
+    <row r="14" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B14" s="2">
+        <v>44696</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B15" s="2">
+        <v>44697</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <v>44680</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="4">
+    <row r="16" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B16" s="2">
+        <v>44698</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
-        <v>44683</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
-        <v>44685</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="4">
+    <row r="17" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B17" s="2">
+        <v>44699</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
-        <v>44690</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
-        <v>44691</v>
-      </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="4"/>
-    </row>
-    <row r="12" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="4"/>
-    </row>
-    <row r="13" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="4"/>
-    </row>
-    <row r="14" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="4"/>
-    </row>
-    <row r="15" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="4"/>
-    </row>
-    <row r="16" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="4"/>
-    </row>
-    <row r="17" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="4"/>
-    </row>
-    <row r="18" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="4"/>
-    </row>
-    <row r="19" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="4"/>
-    </row>
-    <row r="20" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="4"/>
-    </row>
-    <row r="21" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="4"/>
-    </row>
-    <row r="22" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="4"/>
-    </row>
-    <row r="23" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="4"/>
-    </row>
-    <row r="24" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="4"/>
-    </row>
-    <row r="25" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="2"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="4"/>
-    </row>
-    <row r="26" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="2"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="4"/>
-    </row>
-    <row r="27" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="2"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="4"/>
-    </row>
-    <row r="28" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="2"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="4"/>
-    </row>
-    <row r="29" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="2"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="4"/>
-    </row>
-    <row r="30" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="2"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="4"/>
-    </row>
-    <row r="31" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="2"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="4"/>
-    </row>
-    <row r="32" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="2"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="4"/>
-    </row>
-    <row r="33" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="2"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="4"/>
-    </row>
-    <row r="34" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="2"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="4"/>
-    </row>
-    <row r="35" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="2"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="4"/>
-    </row>
-    <row r="36" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="2"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="4"/>
-    </row>
-    <row r="37" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="2"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="4"/>
-    </row>
-    <row r="38" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="2"/>
-      <c r="B38" s="5"/>
-      <c r="C38" s="4"/>
-    </row>
-    <row r="39" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="2"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="4"/>
-    </row>
-    <row r="40" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="2"/>
-      <c r="B40" s="5"/>
-      <c r="C40" s="4"/>
+    <row r="18" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B18" s="2">
+        <v>44700</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B19" s="2">
+        <v>44701</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B20" s="2"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B21" s="2"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B22" s="2"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B23" s="2"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B24" s="2"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B25" s="2"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B26" s="2"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B27" s="2"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="4"/>
+    </row>
+    <row r="28" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B28" s="2"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B29" s="2"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B30" s="2"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B31" s="2"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="4"/>
+    </row>
+    <row r="32" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B32" s="2"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="4"/>
+    </row>
+    <row r="33" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B33" s="2"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="4"/>
+    </row>
+    <row r="34" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B34" s="2"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="4"/>
+    </row>
+    <row r="35" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B35" s="2"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="4"/>
+    </row>
+    <row r="36" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B36" s="2"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="4"/>
+    </row>
+    <row r="37" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B37" s="2"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="4"/>
+    </row>
+    <row r="38" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B38" s="2"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="4"/>
+    </row>
+    <row r="39" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B39" s="2"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="4"/>
+    </row>
+    <row r="40" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B40" s="2"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="4"/>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="D41">
+        <f>SUM(D4:D40)</f>
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Time tracking and error correction of UI
</commit_message>
<xml_diff>
--- a/docs/TimeTracking.xlsx
+++ b/docs/TimeTracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FH\SWEN\TourPlanner_Ortner_Szuesz\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B198BA39-BEAA-407D-B179-AD7D6CDD1FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41ADBC61-7462-4F86-AB2C-2698AB7EB3C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="37220" windowHeight="21820" xr2:uid="{7D11CD6D-A168-461A-B814-780A183E0DF9}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Tour-Planner Ortner &amp; Szüsz</t>
   </si>
@@ -68,9 +68,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Time (h)</t>
-  </si>
-  <si>
     <t>Dependency Injection, update UI when selected tour has changed</t>
   </si>
   <si>
@@ -105,6 +102,18 @@
   </si>
   <si>
     <t>Finished unit testing</t>
+  </si>
+  <si>
+    <t>Style headings and UI elements, started logging</t>
+  </si>
+  <si>
+    <t>Finished logging, error correction, refactoring of ViewModels and Commands</t>
+  </si>
+  <si>
+    <t>Time (h) Sascha</t>
+  </si>
+  <si>
+    <t>Time (h) Viktor</t>
   </si>
 </sst>
 </file>
@@ -157,7 +166,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -208,11 +217,76 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -220,12 +294,38 @@
     <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -542,10 +642,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD90E2B8-0983-41CE-A418-47A70827F2D2}">
-  <dimension ref="B1:D41"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -553,336 +656,314 @@
     <col min="1" max="1" width="4.7265625" customWidth="1"/>
     <col min="2" max="2" width="13.08984375" customWidth="1"/>
     <col min="3" max="3" width="82.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.36328125" customWidth="1"/>
+    <col min="4" max="4" width="11.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="6" t="s">
+    <row r="1" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-    </row>
-    <row r="3" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="3" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B4" s="2">
         <v>44619</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="4">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D4" s="8">
+        <v>5</v>
+      </c>
+      <c r="E4" s="9"/>
+    </row>
+    <row r="5" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B5" s="2">
         <v>44676</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D5" s="8"/>
+      <c r="E5" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B6" s="2">
         <v>44679</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D6" s="8"/>
+      <c r="E6" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B7" s="2">
         <v>44680</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D7" s="9">
+        <v>4</v>
+      </c>
+      <c r="E7" s="9"/>
+    </row>
+    <row r="8" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B8" s="2">
         <v>44683</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D8" s="9">
+        <v>2</v>
+      </c>
+      <c r="E8" s="9"/>
+    </row>
+    <row r="9" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B9" s="2">
         <v>44685</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D9" s="9">
+        <v>4</v>
+      </c>
+      <c r="E9" s="9"/>
+    </row>
+    <row r="10" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B10" s="2">
         <v>44690</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D10" s="8"/>
+      <c r="E10" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B11" s="2">
         <v>44691</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D11" s="8">
+        <v>6</v>
+      </c>
+      <c r="E11" s="9"/>
+    </row>
+    <row r="12" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B12" s="2">
         <v>44692</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="8">
+        <v>6</v>
+      </c>
+      <c r="E12" s="9"/>
+    </row>
+    <row r="13" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B13" s="2">
         <v>44693</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="8">
+        <v>4</v>
+      </c>
+      <c r="E13" s="9"/>
+    </row>
+    <row r="14" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B14" s="2">
         <v>44696</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B15" s="2">
         <v>44697</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B16" s="2">
         <v>44698</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="8">
+        <v>4</v>
+      </c>
+      <c r="E16" s="9"/>
+    </row>
+    <row r="17" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B17" s="2">
         <v>44699</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="8">
+        <v>4</v>
+      </c>
+      <c r="E17" s="9"/>
+    </row>
+    <row r="18" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B18" s="2">
         <v>44700</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C18" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="8"/>
+      <c r="E18" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B19" s="2">
         <v>44701</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" s="4">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C19" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="8">
+        <v>3</v>
+      </c>
+      <c r="E19" s="9"/>
+    </row>
+    <row r="20" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B20" s="2">
         <v>44704</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C20" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="8">
+        <v>8</v>
+      </c>
+      <c r="E20" s="9"/>
+    </row>
+    <row r="21" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B21" s="2">
         <v>44705</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D21" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C21" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B22" s="2">
         <v>44706</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C22" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="8"/>
+      <c r="E22" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B23" s="2">
         <v>44707</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="8">
+        <v>5</v>
+      </c>
+      <c r="E23" s="9"/>
+    </row>
+    <row r="24" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B24" s="2">
+        <v>44708</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="4">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B24" s="2"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="4"/>
-    </row>
-    <row r="25" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B25" s="2"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="4"/>
-    </row>
-    <row r="26" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B26" s="2"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="4"/>
-    </row>
-    <row r="27" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B27" s="2"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="4"/>
-    </row>
-    <row r="28" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B28" s="2"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B29" s="2"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B30" s="2"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="4"/>
-    </row>
-    <row r="31" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B31" s="2"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="4"/>
-    </row>
-    <row r="32" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B32" s="2"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="4"/>
-    </row>
-    <row r="33" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B33" s="2"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="4"/>
-    </row>
-    <row r="34" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B34" s="2"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="4"/>
-    </row>
-    <row r="35" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B35" s="2"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="4"/>
-    </row>
-    <row r="36" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B36" s="2"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="4"/>
-    </row>
-    <row r="37" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B37" s="2"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="4"/>
-    </row>
-    <row r="38" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B38" s="2"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="4"/>
-    </row>
-    <row r="39" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B39" s="2"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="4"/>
-    </row>
-    <row r="40" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B40" s="2"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="4"/>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="D41">
-        <f>SUM(D4:D40)</f>
-        <v>51.5</v>
+      <c r="D24" s="8"/>
+      <c r="E24" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B25" s="2">
+        <v>44709</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="8">
+        <v>8</v>
+      </c>
+      <c r="E25" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B26" s="13">
+        <v>44710</v>
+      </c>
+      <c r="C26" s="14"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="16"/>
+    </row>
+    <row r="27" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B27" s="10"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="12">
+        <f>SUM(D4:D26)</f>
+        <v>63</v>
+      </c>
+      <c r="E27" s="12">
+        <f>SUM(E4:E26)</f>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -890,6 +971,6 @@
     <mergeCell ref="B1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>